<commit_message>
feito melhoria na visualização do estoque de itens induvidualmente
</commit_message>
<xml_diff>
--- a/Estoque_com_codigo_de_barras.xlsx
+++ b/Estoque_com_codigo_de_barras.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raian Satyro\OneDrive\Documentos\Dev\python\estoqueOggi\Projeto-estoque\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C516555-6CF4-48BD-976C-F0F8EB28F80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA96133A-B2AB-4825-8A57-715F61B94951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21450" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23880" yWindow="765" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
   <si>
     <t>Codigo_de_Barras</t>
   </si>
@@ -43,409 +43,421 @@
     <t>rol22208</t>
   </si>
   <si>
+    <t>Rolamento 22208</t>
+  </si>
+  <si>
     <t>rol51104</t>
   </si>
   <si>
+    <t>Rolamento 51104</t>
+  </si>
+  <si>
     <t>rol2207-2RS</t>
   </si>
   <si>
+    <t>Rolamento 2207-2RS</t>
+  </si>
+  <si>
     <t>rol22218-C3</t>
   </si>
   <si>
+    <t>Rolamento 22218-C3</t>
+  </si>
+  <si>
     <t>rol3314A</t>
   </si>
   <si>
+    <t>Rolamento 3314A</t>
+  </si>
+  <si>
     <t>rol22</t>
   </si>
   <si>
+    <t>Rolamento 22</t>
+  </si>
+  <si>
     <t>rol6000-2Z</t>
   </si>
   <si>
+    <t>Rolamento 6000-2Z</t>
+  </si>
+  <si>
     <t>rol6001-2RS-INOX</t>
   </si>
   <si>
+    <t>Rolamento 6001-2RS-INOX</t>
+  </si>
+  <si>
     <t>rol6001-2Z</t>
   </si>
   <si>
+    <t>Rolamento 6001-2Z</t>
+  </si>
+  <si>
     <t>rol6002-2Z</t>
   </si>
   <si>
+    <t>Rolamento 6002-2Z</t>
+  </si>
+  <si>
     <t>rol6003-2Z</t>
   </si>
   <si>
+    <t>Rolamento 6003-2Z</t>
+  </si>
+  <si>
     <t>rol6004-2Z</t>
   </si>
   <si>
+    <t>Rolamento 6004-2Z</t>
+  </si>
+  <si>
     <t>rol6005-2RS</t>
   </si>
   <si>
+    <t>Rolamento 6005-2RS</t>
+  </si>
+  <si>
     <t>rol6005-2RS-INOX</t>
   </si>
   <si>
+    <t>Rolamento 6005-2RS-INOX</t>
+  </si>
+  <si>
     <t>rol6005-2Z</t>
   </si>
   <si>
+    <t>Rolamento 6005-2Z</t>
+  </si>
+  <si>
     <t xml:space="preserve">rol6006-2RS  </t>
   </si>
   <si>
+    <t xml:space="preserve">Rolamento 6006-2RS  </t>
+  </si>
+  <si>
     <t>rol6006-2RS-INOX</t>
   </si>
   <si>
+    <t>Rolamento 6006-2RS-INOX</t>
+  </si>
+  <si>
     <t>rol6006-2Z</t>
   </si>
   <si>
+    <t>Rolamento 6006-2Z</t>
+  </si>
+  <si>
     <t>rol6006-Z-INOX</t>
   </si>
   <si>
+    <t>Rolamento 6006-Z-INOX</t>
+  </si>
+  <si>
     <t>rol6009-2Z</t>
   </si>
   <si>
+    <t>Rolamento 6009-2Z</t>
+  </si>
+  <si>
     <t>rol6010-2Z</t>
   </si>
   <si>
+    <t>Rolamento 6010-2Z</t>
+  </si>
+  <si>
     <t>rol6010-UB</t>
   </si>
   <si>
+    <t>Rolamento 6010-UB</t>
+  </si>
+  <si>
     <t>rol608-2Z</t>
   </si>
   <si>
+    <t>Rolamento 608-2Z</t>
+  </si>
+  <si>
     <t>rol609-Z</t>
   </si>
   <si>
+    <t>Rolamento 609-Z</t>
+  </si>
+  <si>
     <t>rol6201-2RS</t>
   </si>
   <si>
+    <t>Rolamento 6201-2RS</t>
+  </si>
+  <si>
     <t>rol6201-2Z</t>
   </si>
   <si>
+    <t>Rolamento 6201-2Z</t>
+  </si>
+  <si>
     <t>rol6202-2RS-C3</t>
   </si>
   <si>
+    <t>Rolamento 6202-2RS-C3</t>
+  </si>
+  <si>
     <t>rol6202-2Z</t>
   </si>
   <si>
+    <t>Rolamento 6202-2Z</t>
+  </si>
+  <si>
     <t>rol6203-2Z</t>
   </si>
   <si>
+    <t>Rolamento 6203-2Z</t>
+  </si>
+  <si>
     <t>rol6204-2Z</t>
   </si>
   <si>
+    <t>Rolamento 6204-2Z</t>
+  </si>
+  <si>
     <t>rol6205-2Z</t>
   </si>
   <si>
+    <t>Rolamento 6205-2Z</t>
+  </si>
+  <si>
     <t>rol6205-2Z-INOX</t>
   </si>
   <si>
+    <t>Rolamento 6205-2Z-INOX</t>
+  </si>
+  <si>
     <t>rol6206-2Z</t>
   </si>
   <si>
+    <t>Rolamento 6206-2Z</t>
+  </si>
+  <si>
     <t>rol6208-ZZ</t>
   </si>
   <si>
+    <t>Rolamento 6208-ZZ</t>
+  </si>
+  <si>
     <t>rol6209-2Z</t>
   </si>
   <si>
+    <t>Rolamento 6209-2Z</t>
+  </si>
+  <si>
     <t>rol6212-2Z-INOX</t>
   </si>
   <si>
+    <t>Rolamento 6212-2Z-INOX</t>
+  </si>
+  <si>
     <t>rol62202-2RS</t>
   </si>
   <si>
+    <t>Rolamento 62202-2RS</t>
+  </si>
+  <si>
     <t>rol62203-2RS</t>
   </si>
   <si>
+    <t>Rolamento 62203-2RS</t>
+  </si>
+  <si>
     <t>rol6304-2RS-INOX</t>
   </si>
   <si>
+    <t>Rolamento 6304-2RS-INOX</t>
+  </si>
+  <si>
     <t>rol6304-UB</t>
   </si>
   <si>
+    <t>Rolamento 6304-UB</t>
+  </si>
+  <si>
     <t>rol6305-INOX</t>
   </si>
   <si>
+    <t>Rolamento 6305-INOX</t>
+  </si>
+  <si>
     <t>rol6305-2Z</t>
   </si>
   <si>
+    <t>Rolamento 6305-2Z</t>
+  </si>
+  <si>
     <t>rol6306-2Z</t>
   </si>
   <si>
+    <t>Rolamento 6306-2Z</t>
+  </si>
+  <si>
     <t>rol6312-2Z</t>
   </si>
   <si>
+    <t>Rolamento 6312-2Z</t>
+  </si>
+  <si>
     <t>rol6312-C3</t>
   </si>
   <si>
+    <t>Rolamento 6312-C3</t>
+  </si>
+  <si>
     <t>rol6314-2RS</t>
   </si>
   <si>
+    <t>Rolamento 6314-2RS</t>
+  </si>
+  <si>
     <t>rol6801-2RS</t>
   </si>
   <si>
+    <t>Rolamento 6801-2RS</t>
+  </si>
+  <si>
     <t>rol6803-2RS</t>
   </si>
   <si>
+    <t>Rolamento 6803-2RS</t>
+  </si>
+  <si>
     <t>rol6900-Z</t>
   </si>
   <si>
+    <t>Rolamento 6900-Z</t>
+  </si>
+  <si>
     <t>rol698-2RS</t>
   </si>
   <si>
+    <t>Rolamento 698-2RS</t>
+  </si>
+  <si>
     <t>rol698-2Z</t>
   </si>
   <si>
+    <t>Rolamento 698-2Z</t>
+  </si>
+  <si>
     <t>rol7208B</t>
   </si>
   <si>
+    <t>Rolamento 7208B</t>
+  </si>
+  <si>
     <t>rolCF12-BVU</t>
   </si>
   <si>
+    <t>Rolamento CF12-BVU</t>
+  </si>
+  <si>
     <t>rolCF12BUUR</t>
   </si>
   <si>
+    <t>Rolamento CF12BUUR</t>
+  </si>
+  <si>
     <t>rolHF-1616</t>
   </si>
   <si>
+    <t>Rolamento HF-1616</t>
+  </si>
+  <si>
     <t>rolKR26-OPP-A</t>
   </si>
   <si>
+    <t>Rolamento KR26-OPP-A</t>
+  </si>
+  <si>
     <t>rolSB-205</t>
   </si>
   <si>
+    <t>Rolamento SB-205</t>
+  </si>
+  <si>
     <t>rolSB-204</t>
   </si>
   <si>
+    <t>Rolamento SB-204</t>
+  </si>
+  <si>
     <t>rolUC-204</t>
   </si>
   <si>
+    <t>Rolamento UC-204</t>
+  </si>
+  <si>
     <t>rolUC-205</t>
   </si>
   <si>
+    <t>Rolamento UC-205</t>
+  </si>
+  <si>
     <t>rolUC-206</t>
   </si>
   <si>
+    <t>Rolamento UC-206</t>
+  </si>
+  <si>
     <t>rolUC-208</t>
   </si>
   <si>
+    <t>Rolamento UC-208</t>
+  </si>
+  <si>
     <t>rolUC-208-INOX</t>
   </si>
   <si>
+    <t>Rolamento UC-208-INOX</t>
+  </si>
+  <si>
     <t>rolUC-207</t>
   </si>
   <si>
+    <t>Rolamento UC-207</t>
+  </si>
+  <si>
     <t>rolY-204</t>
   </si>
   <si>
+    <t>Rolamento Y-204</t>
+  </si>
+  <si>
     <t>rolY-207</t>
   </si>
   <si>
+    <t>Rolamento Y-207</t>
+  </si>
+  <si>
     <t>rolYAR-205</t>
   </si>
   <si>
+    <t>Rolamento YAR-205</t>
+  </si>
+  <si>
     <t>dis50</t>
   </si>
   <si>
     <t>Disjuntor 50 Amperes</t>
   </si>
   <si>
-    <t>Rolamento 22208</t>
-  </si>
-  <si>
-    <t>Rolamento 51104</t>
-  </si>
-  <si>
-    <t>Rolamento 2207-2RS</t>
-  </si>
-  <si>
-    <t>Rolamento 22218-C3</t>
-  </si>
-  <si>
-    <t>Rolamento 3314A</t>
-  </si>
-  <si>
-    <t>Rolamento 22</t>
-  </si>
-  <si>
-    <t>Rolamento 6000-2Z</t>
-  </si>
-  <si>
-    <t>Rolamento 6001-2RS-INOX</t>
-  </si>
-  <si>
-    <t>Rolamento 6001-2Z</t>
-  </si>
-  <si>
-    <t>Rolamento 6002-2Z</t>
-  </si>
-  <si>
-    <t>Rolamento 6003-2Z</t>
-  </si>
-  <si>
-    <t>Rolamento 6004-2Z</t>
-  </si>
-  <si>
-    <t>Rolamento 6005-2RS</t>
-  </si>
-  <si>
-    <t>Rolamento 6005-2RS-INOX</t>
-  </si>
-  <si>
-    <t>Rolamento 6005-2Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rolamento 6006-2RS  </t>
-  </si>
-  <si>
-    <t>Rolamento 6006-2RS-INOX</t>
-  </si>
-  <si>
-    <t>Rolamento 6006-2Z</t>
-  </si>
-  <si>
-    <t>Rolamento 6006-Z-INOX</t>
-  </si>
-  <si>
-    <t>Rolamento 6009-2Z</t>
-  </si>
-  <si>
-    <t>Rolamento 6010-2Z</t>
-  </si>
-  <si>
-    <t>Rolamento 6010-UB</t>
-  </si>
-  <si>
-    <t>Rolamento 608-2Z</t>
-  </si>
-  <si>
-    <t>Rolamento 609-Z</t>
-  </si>
-  <si>
-    <t>Rolamento 6201-2RS</t>
-  </si>
-  <si>
-    <t>Rolamento 6201-2Z</t>
-  </si>
-  <si>
-    <t>Rolamento 6202-2RS-C3</t>
-  </si>
-  <si>
-    <t>Rolamento 6202-2Z</t>
-  </si>
-  <si>
-    <t>Rolamento 6203-2Z</t>
-  </si>
-  <si>
-    <t>Rolamento 6204-2Z</t>
-  </si>
-  <si>
-    <t>Rolamento 6205-2Z</t>
-  </si>
-  <si>
-    <t>Rolamento 6205-2Z-INOX</t>
-  </si>
-  <si>
-    <t>Rolamento 6206-2Z</t>
-  </si>
-  <si>
-    <t>Rolamento 6208-ZZ</t>
-  </si>
-  <si>
-    <t>Rolamento 6209-2Z</t>
-  </si>
-  <si>
-    <t>Rolamento 6212-2Z-INOX</t>
-  </si>
-  <si>
-    <t>Rolamento 62202-2RS</t>
-  </si>
-  <si>
-    <t>Rolamento 62203-2RS</t>
-  </si>
-  <si>
-    <t>Rolamento 6304-2RS-INOX</t>
-  </si>
-  <si>
-    <t>Rolamento 6304-UB</t>
-  </si>
-  <si>
-    <t>Rolamento 6305-INOX</t>
-  </si>
-  <si>
-    <t>Rolamento 6305-2Z</t>
-  </si>
-  <si>
-    <t>Rolamento 6306-2Z</t>
-  </si>
-  <si>
-    <t>Rolamento 6312-2Z</t>
-  </si>
-  <si>
-    <t>Rolamento 6312-C3</t>
-  </si>
-  <si>
-    <t>Rolamento 6314-2RS</t>
-  </si>
-  <si>
-    <t>Rolamento 6801-2RS</t>
-  </si>
-  <si>
-    <t>Rolamento 6803-2RS</t>
-  </si>
-  <si>
-    <t>Rolamento 6900-Z</t>
-  </si>
-  <si>
-    <t>Rolamento 698-2RS</t>
-  </si>
-  <si>
-    <t>Rolamento 698-2Z</t>
-  </si>
-  <si>
-    <t>Rolamento 7208B</t>
-  </si>
-  <si>
-    <t>Rolamento CF12-BVU</t>
-  </si>
-  <si>
-    <t>Rolamento CF12BUUR</t>
-  </si>
-  <si>
-    <t>Rolamento HF-1616</t>
-  </si>
-  <si>
-    <t>Rolamento KR26-OPP-A</t>
-  </si>
-  <si>
-    <t>Rolamento SB-205</t>
-  </si>
-  <si>
-    <t>Rolamento SB-204</t>
-  </si>
-  <si>
-    <t>Rolamento UC-204</t>
-  </si>
-  <si>
-    <t>Rolamento UC-205</t>
-  </si>
-  <si>
-    <t>Rolamento UC-206</t>
-  </si>
-  <si>
-    <t>Rolamento UC-208</t>
-  </si>
-  <si>
-    <t>Rolamento UC-208-INOX</t>
-  </si>
-  <si>
-    <t>Rolamento UC-207</t>
-  </si>
-  <si>
-    <t>Rolamento Y-204</t>
-  </si>
-  <si>
-    <t>Rolamento Y-207</t>
-  </si>
-  <si>
-    <t>Rolamento YAR-205</t>
+    <t>dis21</t>
+  </si>
+  <si>
+    <t>Disjuntor 21 amperes</t>
+  </si>
+  <si>
+    <t>pneu8</t>
+  </si>
+  <si>
+    <t>conexão reta de 8mm</t>
   </si>
 </sst>
 </file>
@@ -466,7 +478,9 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="8"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -512,9 +526,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -817,16 +829,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -852,8 +861,8 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>75</v>
+      <c r="B2" t="s">
+        <v>7</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -870,10 +879,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>76</v>
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
       </c>
       <c r="C3">
         <v>6</v>
@@ -890,10 +899,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>77</v>
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -910,10 +919,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>78</v>
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -930,10 +939,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>79</v>
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -950,13 +959,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>80</v>
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -970,10 +979,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>81</v>
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -990,10 +999,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>82</v>
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
       </c>
       <c r="C9">
         <v>41</v>
@@ -1010,10 +1019,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>83</v>
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1030,10 +1039,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>84</v>
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -1050,10 +1059,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>85</v>
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
       </c>
       <c r="C12">
         <v>18</v>
@@ -1070,10 +1079,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>86</v>
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
       </c>
       <c r="C13">
         <v>15</v>
@@ -1090,10 +1099,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>87</v>
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1110,10 +1119,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>88</v>
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
       </c>
       <c r="C15">
         <v>8</v>
@@ -1130,10 +1139,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>89</v>
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
       </c>
       <c r="C16">
         <v>11</v>
@@ -1150,10 +1159,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>90</v>
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
       </c>
       <c r="C17">
         <v>7</v>
@@ -1170,10 +1179,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>91</v>
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -1190,10 +1199,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>92</v>
+        <v>40</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
       </c>
       <c r="C19">
         <v>5</v>
@@ -1210,10 +1219,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>93</v>
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
       </c>
       <c r="C20">
         <v>4</v>
@@ -1230,10 +1239,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>94</v>
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>45</v>
       </c>
       <c r="C21">
         <v>7</v>
@@ -1250,10 +1259,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>95</v>
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -1270,10 +1279,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>96</v>
+        <v>48</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1290,10 +1299,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>97</v>
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
       </c>
       <c r="C24">
         <v>21</v>
@@ -1310,10 +1319,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>98</v>
+        <v>52</v>
+      </c>
+      <c r="B25" t="s">
+        <v>53</v>
       </c>
       <c r="C25">
         <v>9</v>
@@ -1330,10 +1339,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>99</v>
+        <v>54</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
       </c>
       <c r="C26">
         <v>8</v>
@@ -1350,10 +1359,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>100</v>
+        <v>56</v>
+      </c>
+      <c r="B27" t="s">
+        <v>57</v>
       </c>
       <c r="C27">
         <v>16</v>
@@ -1370,10 +1379,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>101</v>
+        <v>58</v>
+      </c>
+      <c r="B28" t="s">
+        <v>59</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -1390,10 +1399,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>102</v>
+        <v>60</v>
+      </c>
+      <c r="B29" t="s">
+        <v>61</v>
       </c>
       <c r="C29">
         <v>8</v>
@@ -1410,10 +1419,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>103</v>
+        <v>62</v>
+      </c>
+      <c r="B30" t="s">
+        <v>63</v>
       </c>
       <c r="C30">
         <v>9</v>
@@ -1430,10 +1439,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>104</v>
+        <v>64</v>
+      </c>
+      <c r="B31" t="s">
+        <v>65</v>
       </c>
       <c r="C31">
         <v>9</v>
@@ -1450,10 +1459,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>105</v>
+        <v>66</v>
+      </c>
+      <c r="B32" t="s">
+        <v>67</v>
       </c>
       <c r="C32">
         <v>16</v>
@@ -1470,10 +1479,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>106</v>
+        <v>68</v>
+      </c>
+      <c r="B33" t="s">
+        <v>69</v>
       </c>
       <c r="C33">
         <v>8</v>
@@ -1490,10 +1499,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>107</v>
+        <v>70</v>
+      </c>
+      <c r="B34" t="s">
+        <v>71</v>
       </c>
       <c r="C34">
         <v>4</v>
@@ -1510,10 +1519,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>39</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>108</v>
+        <v>72</v>
+      </c>
+      <c r="B35" t="s">
+        <v>73</v>
       </c>
       <c r="C35">
         <v>4</v>
@@ -1530,10 +1539,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>40</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>109</v>
+        <v>74</v>
+      </c>
+      <c r="B36" t="s">
+        <v>75</v>
       </c>
       <c r="C36">
         <v>8</v>
@@ -1550,10 +1559,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>110</v>
+        <v>76</v>
+      </c>
+      <c r="B37" t="s">
+        <v>77</v>
       </c>
       <c r="C37">
         <v>4</v>
@@ -1570,10 +1579,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>42</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>111</v>
+        <v>78</v>
+      </c>
+      <c r="B38" t="s">
+        <v>79</v>
       </c>
       <c r="C38">
         <v>6</v>
@@ -1590,10 +1599,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>112</v>
+        <v>80</v>
+      </c>
+      <c r="B39" t="s">
+        <v>81</v>
       </c>
       <c r="C39">
         <v>12</v>
@@ -1610,10 +1619,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>113</v>
+        <v>82</v>
+      </c>
+      <c r="B40" t="s">
+        <v>83</v>
       </c>
       <c r="C40">
         <v>45</v>
@@ -1630,10 +1639,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>114</v>
+        <v>84</v>
+      </c>
+      <c r="B41" t="s">
+        <v>85</v>
       </c>
       <c r="C41">
         <v>24</v>
@@ -1650,10 +1659,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>115</v>
+        <v>86</v>
+      </c>
+      <c r="B42" t="s">
+        <v>87</v>
       </c>
       <c r="C42">
         <v>9</v>
@@ -1670,10 +1679,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>116</v>
+        <v>88</v>
+      </c>
+      <c r="B43" t="s">
+        <v>89</v>
       </c>
       <c r="C43">
         <v>17</v>
@@ -1690,10 +1699,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>117</v>
+        <v>90</v>
+      </c>
+      <c r="B44" t="s">
+        <v>91</v>
       </c>
       <c r="C44">
         <v>10</v>
@@ -1710,10 +1719,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>118</v>
+        <v>92</v>
+      </c>
+      <c r="B45" t="s">
+        <v>93</v>
       </c>
       <c r="C45">
         <v>2</v>
@@ -1730,10 +1739,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>119</v>
+        <v>94</v>
+      </c>
+      <c r="B46" t="s">
+        <v>95</v>
       </c>
       <c r="C46">
         <v>2</v>
@@ -1750,10 +1759,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>51</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>120</v>
+        <v>96</v>
+      </c>
+      <c r="B47" t="s">
+        <v>97</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -1770,10 +1779,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>52</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>121</v>
+        <v>98</v>
+      </c>
+      <c r="B48" t="s">
+        <v>99</v>
       </c>
       <c r="C48">
         <v>11</v>
@@ -1790,10 +1799,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>53</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>122</v>
+        <v>100</v>
+      </c>
+      <c r="B49" t="s">
+        <v>101</v>
       </c>
       <c r="C49">
         <v>18</v>
@@ -1810,10 +1819,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>54</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>123</v>
+        <v>102</v>
+      </c>
+      <c r="B50" t="s">
+        <v>103</v>
       </c>
       <c r="C50">
         <v>49</v>
@@ -1830,10 +1839,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>55</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>124</v>
+        <v>104</v>
+      </c>
+      <c r="B51" t="s">
+        <v>105</v>
       </c>
       <c r="C51">
         <v>6</v>
@@ -1850,10 +1859,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>125</v>
+        <v>106</v>
+      </c>
+      <c r="B52" t="s">
+        <v>107</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -1870,10 +1879,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>57</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>126</v>
+        <v>108</v>
+      </c>
+      <c r="B53" t="s">
+        <v>109</v>
       </c>
       <c r="C53">
         <v>8</v>
@@ -1890,10 +1899,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>58</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>127</v>
+        <v>110</v>
+      </c>
+      <c r="B54" t="s">
+        <v>111</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -1910,10 +1919,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>59</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>128</v>
+        <v>112</v>
+      </c>
+      <c r="B55" t="s">
+        <v>113</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -1930,10 +1939,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>60</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>129</v>
+        <v>114</v>
+      </c>
+      <c r="B56" t="s">
+        <v>115</v>
       </c>
       <c r="C56">
         <v>15</v>
@@ -1950,10 +1959,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>61</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>130</v>
+        <v>116</v>
+      </c>
+      <c r="B57" t="s">
+        <v>117</v>
       </c>
       <c r="C57">
         <v>3</v>
@@ -1970,10 +1979,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>62</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>131</v>
+        <v>118</v>
+      </c>
+      <c r="B58" t="s">
+        <v>119</v>
       </c>
       <c r="C58">
         <v>8</v>
@@ -1990,10 +1999,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>63</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>132</v>
+        <v>120</v>
+      </c>
+      <c r="B59" t="s">
+        <v>121</v>
       </c>
       <c r="C59">
         <v>7</v>
@@ -2010,10 +2019,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>64</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>133</v>
+        <v>122</v>
+      </c>
+      <c r="B60" t="s">
+        <v>123</v>
       </c>
       <c r="C60">
         <v>11</v>
@@ -2030,10 +2039,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>65</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>134</v>
+        <v>124</v>
+      </c>
+      <c r="B61" t="s">
+        <v>125</v>
       </c>
       <c r="C61">
         <v>6</v>
@@ -2050,10 +2059,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>66</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>135</v>
+        <v>126</v>
+      </c>
+      <c r="B62" t="s">
+        <v>127</v>
       </c>
       <c r="C62">
         <v>6</v>
@@ -2070,10 +2079,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>67</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>136</v>
+        <v>128</v>
+      </c>
+      <c r="B63" t="s">
+        <v>129</v>
       </c>
       <c r="C63">
         <v>10</v>
@@ -2090,10 +2099,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>68</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>137</v>
+        <v>130</v>
+      </c>
+      <c r="B64" t="s">
+        <v>131</v>
       </c>
       <c r="C64">
         <v>2</v>
@@ -2110,10 +2119,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>69</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
+      </c>
+      <c r="B65" t="s">
+        <v>133</v>
       </c>
       <c r="C65">
         <v>6</v>
@@ -2130,10 +2139,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>70</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
+      </c>
+      <c r="B66" t="s">
+        <v>135</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -2150,10 +2159,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>71</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
+      </c>
+      <c r="B67" t="s">
+        <v>137</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -2170,10 +2179,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>72</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
+      </c>
+      <c r="B68" t="s">
+        <v>139</v>
       </c>
       <c r="C68">
         <v>9</v>
@@ -2190,10 +2199,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>73</v>
+        <v>140</v>
       </c>
       <c r="B69" t="s">
-        <v>74</v>
+        <v>141</v>
       </c>
       <c r="C69">
         <v>2</v>
@@ -2208,8 +2217,50 @@
         <v>0</v>
       </c>
     </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>142</v>
+      </c>
+      <c r="B70" t="s">
+        <v>143</v>
+      </c>
+      <c r="C70">
+        <v>6</v>
+      </c>
+      <c r="D70">
+        <v>4</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>144</v>
+      </c>
+      <c r="B71" t="s">
+        <v>145</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>5</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C72" s="2"/>
+    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>